<commit_message>
Updated cases for Product Add to Cart and Verify
</commit_message>
<xml_diff>
--- a/code/src/test/Resources/SampleTestData/website_sample_data.xlsx
+++ b/code/src/test/Resources/SampleTestData/website_sample_data.xlsx
@@ -43,7 +43,7 @@
     <t xml:space="preserve">qty</t>
   </si>
   <si>
-    <t xml:space="preserve">boon</t>
+    <t xml:space="preserve">carters</t>
   </si>
   <si>
     <t xml:space="preserve">Clothing</t>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Rompers &amp; Onesies</t>
   </si>
   <si>
-    <t xml:space="preserve">Wayfarer Messenger Bag</t>
+    <t xml:space="preserve">BOON Star Drain Cover</t>
   </si>
   <si>
     <t xml:space="preserve">shorts</t>

</xml_diff>